<commit_message>
Ajout description code implementer dans rapport
Correction dans excel de mauvaise donnee (difference non significative)
</commit_message>
<xml_diff>
--- a/TestA.xlsx
+++ b/TestA.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="TestA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -714,106 +714,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>214106</c:v>
+                  <c:v>212641</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>185575</c:v>
+                  <c:v>185868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153781</c:v>
+                  <c:v>155865</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>126727</c:v>
+                  <c:v>129794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98662</c:v>
+                  <c:v>103915</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75179</c:v>
+                  <c:v>84886</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31033</c:v>
+                  <c:v>39657</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31530</c:v>
+                  <c:v>39522</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29746</c:v>
+                  <c:v>37664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27287</c:v>
+                  <c:v>35522</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26494</c:v>
+                  <c:v>34923</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26841</c:v>
+                  <c:v>35391</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26721</c:v>
+                  <c:v>35433</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27325</c:v>
+                  <c:v>36167</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28032</c:v>
+                  <c:v>36947</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28915</c:v>
+                  <c:v>37926</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28887</c:v>
+                  <c:v>37888</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29475</c:v>
+                  <c:v>38463</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29871</c:v>
+                  <c:v>38797</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30279</c:v>
+                  <c:v>39137</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30636</c:v>
+                  <c:v>39504</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30750</c:v>
+                  <c:v>39549</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31093</c:v>
+                  <c:v>39889</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31296</c:v>
+                  <c:v>40049</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31398</c:v>
+                  <c:v>40090</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>31602</c:v>
+                  <c:v>40261</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="69984640"/>
-        <c:axId val="79981184"/>
+        <c:axId val="79051392"/>
+        <c:axId val="79081856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69984640"/>
+        <c:axId val="79051392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79981184"/>
+        <c:crossAx val="79081856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79981184"/>
+        <c:axId val="79081856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +821,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69984640"/>
+        <c:crossAx val="79051392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -834,7 +834,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1041,23 +1041,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="71529600"/>
-        <c:axId val="71462272"/>
+        <c:axId val="36930304"/>
+        <c:axId val="36931840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71529600"/>
+        <c:axId val="36930304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71462272"/>
+        <c:crossAx val="36931840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71462272"/>
+        <c:axId val="36931840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1065,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71529600"/>
+        <c:crossAx val="36930304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1078,7 +1078,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1486,7 +1486,7 @@
         <v>11380</v>
       </c>
       <c r="F2" s="1">
-        <v>214106</v>
+        <v>212641</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1506,7 +1506,7 @@
         <v>11380</v>
       </c>
       <c r="F3" s="1">
-        <v>185575</v>
+        <v>185868</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1526,7 +1526,7 @@
         <v>11380</v>
       </c>
       <c r="F4" s="1">
-        <v>153781</v>
+        <v>155865</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1546,7 +1546,7 @@
         <v>11380</v>
       </c>
       <c r="F5" s="1">
-        <v>126727</v>
+        <v>129794</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1566,7 +1566,7 @@
         <v>11380</v>
       </c>
       <c r="F6" s="1">
-        <v>98662</v>
+        <v>103915</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1586,7 +1586,7 @@
         <v>11380</v>
       </c>
       <c r="F7" s="1">
-        <v>75179</v>
+        <v>84886</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1606,7 +1606,7 @@
         <v>11380</v>
       </c>
       <c r="F8" s="1">
-        <v>31033</v>
+        <v>39657</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1626,7 +1626,7 @@
         <v>11694</v>
       </c>
       <c r="F9" s="1">
-        <v>31530</v>
+        <v>39522</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1646,7 +1646,7 @@
         <v>12000</v>
       </c>
       <c r="F10" s="1">
-        <v>29746</v>
+        <v>37664</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1666,7 +1666,7 @@
         <v>12102</v>
       </c>
       <c r="F11" s="1">
-        <v>27287</v>
+        <v>35522</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1686,7 +1686,7 @@
         <v>12192</v>
       </c>
       <c r="F12" s="1">
-        <v>26494</v>
+        <v>34923</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1706,7 +1706,7 @@
         <v>12292</v>
       </c>
       <c r="F13" s="1">
-        <v>26841</v>
+        <v>35391</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1726,7 +1726,7 @@
         <v>12356</v>
       </c>
       <c r="F14" s="1">
-        <v>26721</v>
+        <v>35433</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1746,7 +1746,7 @@
         <v>12410</v>
       </c>
       <c r="F15" s="1">
-        <v>27325</v>
+        <v>36167</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1766,7 +1766,7 @@
         <v>12430</v>
       </c>
       <c r="F16" s="1">
-        <v>28032</v>
+        <v>36947</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1786,7 +1786,7 @@
         <v>12456</v>
       </c>
       <c r="F17" s="1">
-        <v>28915</v>
+        <v>37926</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1806,7 +1806,7 @@
         <v>12546</v>
       </c>
       <c r="F18" s="1">
-        <v>28887</v>
+        <v>37888</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1826,7 +1826,7 @@
         <v>12588</v>
       </c>
       <c r="F19" s="1">
-        <v>29475</v>
+        <v>38463</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1846,7 +1846,7 @@
         <v>12670</v>
       </c>
       <c r="F20" s="1">
-        <v>29871</v>
+        <v>38797</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1866,7 +1866,7 @@
         <v>12756</v>
       </c>
       <c r="F21" s="1">
-        <v>30279</v>
+        <v>39137</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1886,7 +1886,7 @@
         <v>12786</v>
       </c>
       <c r="F22" s="1">
-        <v>30636</v>
+        <v>39504</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1906,7 +1906,7 @@
         <v>12890</v>
       </c>
       <c r="F23" s="1">
-        <v>30750</v>
+        <v>39549</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1926,7 +1926,7 @@
         <v>12948</v>
       </c>
       <c r="F24" s="1">
-        <v>31093</v>
+        <v>39889</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1946,7 +1946,7 @@
         <v>13000</v>
       </c>
       <c r="F25" s="1">
-        <v>31296</v>
+        <v>40049</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1966,7 +1966,7 @@
         <v>13054</v>
       </c>
       <c r="F26" s="1">
-        <v>31398</v>
+        <v>40090</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1986,7 +1986,7 @@
         <v>13082</v>
       </c>
       <c r="F27" s="1">
-        <v>31602</v>
+        <v>40261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>